<commit_message>
Refactor Player's Scripts Structure
Add interface IPlayerBehaviour, IPlayerAction, IPlayerAttack
Add class CSVUtil
-Extract CSV file to Dictionary List

Add class AttackManager,
- Parse CSVUtil's Dictionary List and allocate value to SkillInfo List

Add class AttackController, Attack
Add class PlayerAction, PlayerNormal
Add class InputManager
Remove script PlayerController, PlayerFSM
</commit_message>
<xml_diff>
--- a/DeathHand2D/Assets/Resources/SkillTable.xlsx
+++ b/DeathHand2D/Assets/Resources/SkillTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\GameProject\OnePunchCone\DeathHand2D\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A819A2E-0D4E-4BA9-8A6A-55BFD8AAFE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4460B1-1F75-4F72-9161-A1BDE0B144E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84D5EB44-B505-4882-AF98-2F2755CF33CF}"/>
   </bookViews>
@@ -3731,7 +3731,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>